<commit_message>
Typo in Input file
</commit_message>
<xml_diff>
--- a/Inputs/Inputs.xlsx
+++ b/Inputs/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\COVID-30\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD0C133-32ED-4046-94FD-5D8875505FBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C11426-AEC8-4B51-9A4E-EEB4C4296056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5610" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="5" r:id="rId1"/>
@@ -464,9 +464,6 @@
     <t>y_16</t>
   </si>
   <si>
-    <t>UnusefulIO</t>
-  </si>
-  <si>
     <t>GDP</t>
   </si>
   <si>
@@ -531,6 +528,9 @@
   </si>
   <si>
     <t>Trend</t>
+  </si>
+  <si>
+    <t>NoPrefChange</t>
   </si>
 </sst>
 </file>
@@ -874,11 +874,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD5A7D4-04A2-483C-82E8-978258BC79BD}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,52 +924,52 @@
         <v>136</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
         <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" t="s">
         <v>146</v>
-      </c>
-      <c r="B5" t="s">
-        <v>147</v>
       </c>
       <c r="C5" t="s">
         <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
         <v>161</v>
-      </c>
-      <c r="B6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -982,10 +982,10 @@
   <dimension ref="A1:BI132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AS3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AU1" sqref="AU1:BI1"/>
+      <selection pane="bottomRight" activeCell="AX21" sqref="AX21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49931,7 +49931,7 @@
         <v>2030</v>
       </c>
       <c r="W1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -54775,7 +54775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7406A56-82DD-4C01-B6DD-FF90907FE045}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -55046,7 +55046,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C14"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -55064,7 +55064,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="4">
         <v>1.2607352267624742E-2</v>
@@ -55086,7 +55086,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" s="4">
         <v>1.71178550410469E-2</v>
@@ -55097,7 +55097,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="4">
         <v>2.3471366192929773E-2</v>
@@ -55108,7 +55108,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B6" s="4">
         <v>2.4252181522912513E-2</v>
@@ -55119,7 +55119,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B7" s="4">
         <v>3.8087429941938262E-3</v>
@@ -55130,7 +55130,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" s="4">
         <v>1.4188676766056637E-2</v>
@@ -55141,7 +55141,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" s="4">
         <v>5.1004706653938255E-2</v>
@@ -55152,7 +55152,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B10" s="4">
         <v>0.76786990015477408</v>
@@ -55163,7 +55163,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B11" s="4">
         <v>6.2828481650819687E-3</v>
@@ -55174,7 +55174,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B12" s="4">
         <v>1.5966539367883028E-2</v>
@@ -55185,7 +55185,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B13" s="4">
         <v>1.2050260810599719E-2</v>
@@ -55196,7 +55196,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B14" s="4">
         <v>3.1937508515150069E-3</v>

</xml_diff>

<commit_message>
Option for printing svg included in the paper
Also additional analysis on intermediate results is added.
</commit_message>
<xml_diff>
--- a/Inputs/Inputs.xlsx
+++ b/Inputs/Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\COVID-30\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\COVID-19_impact_on_Italian_GDP\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D833360-13FF-4975-95BC-C10922C24F78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBB3A6C-E113-453B-B62C-3CD5467799C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="5" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="y_pt" sheetId="3" r:id="rId3"/>
     <sheet name="y_fx" sheetId="10" r:id="rId4"/>
     <sheet name="Projected Trends" sheetId="4" r:id="rId5"/>
-    <sheet name="GDP" sheetId="7" r:id="rId6"/>
-    <sheet name="GDP_old" sheetId="9" r:id="rId7"/>
-    <sheet name="Aggregated GDP shares 16 vs 14" sheetId="6" r:id="rId8"/>
+    <sheet name="Aggregated Projected Trends" sheetId="11" r:id="rId6"/>
+    <sheet name="GDP" sheetId="7" r:id="rId7"/>
+    <sheet name="GDP_old" sheetId="9" r:id="rId8"/>
+    <sheet name="Aggregated GDP shares 16 vs 14" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="179">
   <si>
     <t>Products of agriculture, hunting and related services</t>
   </si>
@@ -531,13 +532,59 @@
   <si>
     <t>It contains the level of total Italian GDP for every scenario-year. Input from Economic model.</t>
   </si>
+  <si>
+    <t>Other sectors - commodity</t>
+  </si>
+  <si>
+    <t>Mining - commodity</t>
+  </si>
+  <si>
+    <t>Food, beverages &amp; tobacco - commodity</t>
+  </si>
+  <si>
+    <t>Textile &amp; leather - commodity</t>
+  </si>
+  <si>
+    <t>Wood &amp; wood products - commodity</t>
+  </si>
+  <si>
+    <t>Paper, pulp &amp; printing - commodity</t>
+  </si>
+  <si>
+    <t>Chemicals - commodity</t>
+  </si>
+  <si>
+    <t>Non-metallic minerals - commodity</t>
+  </si>
+  <si>
+    <t>Metals - commodity</t>
+  </si>
+  <si>
+    <t>Other - commodity</t>
+  </si>
+  <si>
+    <t>Machinery - commodity</t>
+  </si>
+  <si>
+    <t>Transport equipment - commodity</t>
+  </si>
+  <si>
+    <t>Utilities - commodity</t>
+  </si>
+  <si>
+    <t>Construction - commodity</t>
+  </si>
+  <si>
+    <t>From 20 to 30</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -576,10 +623,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -590,7 +646,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -600,13 +656,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normale 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -617,6 +686,3058 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Share of industrial products in final</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> consumption by year</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mining - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$3:$R$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>5.4481243884379896E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.56548966737915E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0429787162539802E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0429787162539802E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.57472346726347E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.57876002672824E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Food, beverages &amp; tobacco - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$4:$R$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>4.8846235302194098E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8404089721199903E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8991625293539301E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8991625293539301E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9558206288724801E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.01049496748395E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0571633294625197E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.10107148466186E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.1434041444659198E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.1801320035831898E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.2096315032423797E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.2380205672519303E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.2647531736045299E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.2896244885395599E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.3135964996010102E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.3346940945673903E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.3530976418969797E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Textile &amp; leather - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$5:$R$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>3.5283825703161902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6715395009672698E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5997312302103998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5997312302103998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5304807000391597E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4636548275199797E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.39501683915008E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3281573297978401E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2636968474290103E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1989688226331803E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1330314759766602E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.06957617753165E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.00811822754267E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.94840953327179E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8908598024567599E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.8342792029388601E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.7787053299524699E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wood &amp; wood products - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$6:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1.3866633602674101E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6109333596220101E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.47606050218053E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.47606050218053E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.34599351244962E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2204805372677599E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0979568091240199E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.7965274351189411E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6559361849834196E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.5495561388647504E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.4758284836130997E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.4425186483300896E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.4468734709879099E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.4869808302601698E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5617962527078902E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.66883783543993E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.0738925815293907E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Paper, pulp &amp; printing - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$7:$R$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>5.1947908548329999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0770532380682697E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9430921827453402E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9430921827453402E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8139527150107197E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6893347866469801E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.56433607542963E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5013499699016399E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4406239073833198E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.3785621649348903E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.3138572201904604E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2515879329379303E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.1911356518326299E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.1321977148234199E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.0753908720161502E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.0190774769251897E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.9633313878154599E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Chemicals - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$8:$R$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>4.51007615360981E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3538240914059098E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0377147041685803E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0377147041685803E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7328787920488798E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4387160505910001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1508596468086299E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8727965824996399E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6047108692186301E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.42354281728057E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3595194192137198E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2979060235009899E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2383107605520799E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.18052534585602E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.1248293521418299E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.0703263581689502E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.0170325096472E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Non-metallic minerals - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$9:$R$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1.44629210147961E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3910542780015901E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4220137469831E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4220137469831E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.45187438243776E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4806895122757799E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5066883868955799E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.53142554304645E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.55527509015451E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.57703192312224E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5961944068481601E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6146355663038299E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6322070178052501E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6488611140134401E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.66491302681194E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6797578395370501E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.69345939107097E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Metals - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$10:$R$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2.60868658707736E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5091465557896299E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4595021621217499E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4595021621217499E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4116211221958901E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3654165334041698E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3179945971375199E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2718072267962901E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.22727713376407E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1825838955700401E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.13708532691387E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.09329943925998E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.05089463725374E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0097009144628E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9699966856760901E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9309703368911899E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8926470704058802E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Other - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$11:$R$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>5.5668083466623497E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7776350391532498E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7927073756841301E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.7927073756841301E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.80723564408233E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8212552365605803E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8277345796159501E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.83275138186473E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.8375881731609701E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.8376198711893902E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.8310456348625202E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.8247188693900803E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.8179544560930503E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.8104640280925102E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.8032444410560602E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.7940840343695003E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.7831511555778398E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Machinery - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$12:$R$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>5.01683262158387E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8942553419554398E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9017836183847301E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9017836183847301E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.90904686019095E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9160557952824001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9168688482966703E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9166170017657503E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.91637419189438E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9122400177978198E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.9027020040477397E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8935230252174798E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.8841195461002899E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.8742431234250198E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.8647238151682003E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.8537019761176303E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.8413157547805202E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Transport equipment - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$13:$R$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>3.5222740409149897E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9350890184148501E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3610745841196799E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3610745841196799E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7718731234100399E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1682884396510698E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5443483054485203E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.9055797212069099E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.2538495714070996E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5846155289318697E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.8956161029791102E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.1949098301825595E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4822820417572405E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.7578675632137495E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.0234883872831606E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.2765367487161096E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.5174817386557702E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Utilities - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$14:$R$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1.5328670694862901E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6550341974918201E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7451522681676799E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7451522681676799E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.83205331359735E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9159117067289001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9944690425740201E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.069752678852E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1423350168914699E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2106038431750501E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2738296996887501E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.3346755753260701E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.39299721359078E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.4487803699201598E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.50254650347859E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5534347564824901E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6015665013880099E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Aggregated Projected Trends'!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Construction - commodity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$1:$R$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Aggregated Projected Trends'!$B$15:$R$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>6.6809854973505306E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2245255791008203E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0548112478828797E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0548112478828797E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8911428240930201E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7332048964475101E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5739512034445299E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.4193089181475702E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.2702154473543102E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.1223107017573898E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.9741174759520702E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8315026173349901E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.6936153162248702E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.55999674548455E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.4312095919235003E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.3053637858884199E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.18248216233724E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-DEB2-4633-AADB-7882A9105164}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="699324592"/>
+        <c:axId val="699324920"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Aggregated Projected Trends'!$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Other sectors - commodity</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Aggregated Projected Trends'!$B$1:$R$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="17"/>
+                      <c:pt idx="0">
+                        <c:v>2014</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2015</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2016</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2017</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2018</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2020</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2021</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2022</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2023</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>2024</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>2025</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2026</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>2027</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>2028</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2029</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>2030</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Aggregated Projected Trends'!$B$2:$R$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0%</c:formatCode>
+                      <c:ptCount val="17"/>
+                      <c:pt idx="0">
+                        <c:v>0.59499213620945501</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.596221397990923</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.59780133392804902</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.59780133392804902</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.59932505639559497</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.60079542901395699</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.60148675932710405</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.60202631860019395</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.60254651761671296</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.60256998797076899</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.60191082943419605</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.601276483289232</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.60071165309582097</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.60023437193935303</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.59977434844673905</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.59948254740275297</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.59934653712923802</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-DEB2-4633-AADB-7882A9105164}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="699324592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="699324920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="699324920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="699324592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3338</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>37865</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>327422</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11784EAF-97A4-4DC4-9A2C-207F830F51D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -84880,16 +88001,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P21" sqref="P21"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="155.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -89801,6 +92922,954 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6EECC1-2415-4043-B268-41F763A9307C}">
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="T19" sqref="T19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="18" width="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>2014</v>
+      </c>
+      <c r="C1">
+        <v>2015</v>
+      </c>
+      <c r="D1" s="14">
+        <v>2016</v>
+      </c>
+      <c r="E1" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F1" s="2">
+        <v>2018</v>
+      </c>
+      <c r="G1" s="2">
+        <v>2019</v>
+      </c>
+      <c r="H1" s="2">
+        <v>2020</v>
+      </c>
+      <c r="I1" s="2">
+        <v>2021</v>
+      </c>
+      <c r="J1" s="2">
+        <v>2022</v>
+      </c>
+      <c r="K1" s="2">
+        <v>2023</v>
+      </c>
+      <c r="L1" s="2">
+        <v>2024</v>
+      </c>
+      <c r="M1" s="2">
+        <v>2025</v>
+      </c>
+      <c r="N1" s="2">
+        <v>2026</v>
+      </c>
+      <c r="O1" s="2">
+        <v>2027</v>
+      </c>
+      <c r="P1" s="2">
+        <v>2028</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>2029</v>
+      </c>
+      <c r="R1" s="2">
+        <v>2030</v>
+      </c>
+      <c r="S1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.59499213620945501</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.596221397990923</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0.59780133392804902</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0.59780133392804902</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.59932505639559497</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.60079542901395699</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0.60148675932710405</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0.60202631860019395</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0.60254651761671296</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0.60256998797076899</v>
+      </c>
+      <c r="L2" s="11">
+        <v>0.60191082943419605</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0.601276483289232</v>
+      </c>
+      <c r="N2" s="11">
+        <v>0.60071165309582097</v>
+      </c>
+      <c r="O2" s="11">
+        <v>0.60023437193935303</v>
+      </c>
+      <c r="P2" s="11">
+        <v>0.59977434844673905</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>0.59948254740275297</v>
+      </c>
+      <c r="R2" s="11">
+        <v>0.59934653712923802</v>
+      </c>
+      <c r="S2" s="10">
+        <f>(R2-H2)/H2</f>
+        <v>-3.5582199685664537E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="9">
+        <v>5.4481243884379896E-3</v>
+      </c>
+      <c r="C3" s="9">
+        <v>4.56548966737915E-3</v>
+      </c>
+      <c r="D3" s="13">
+        <v>3.0429787162539802E-3</v>
+      </c>
+      <c r="E3" s="9">
+        <v>3.0429787162539802E-3</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1.57472346726347E-3</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1.57876002672824E-4</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0</v>
+      </c>
+      <c r="N3" s="9">
+        <v>0</v>
+      </c>
+      <c r="O3" s="9">
+        <v>0</v>
+      </c>
+      <c r="P3" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>0</v>
+      </c>
+      <c r="R3" s="9">
+        <v>0</v>
+      </c>
+      <c r="S3" s="10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="9">
+        <v>4.8846235302194098E-2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>4.8404089721199903E-2</v>
+      </c>
+      <c r="D4" s="13">
+        <v>4.8991625293539301E-2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>4.8991625293539301E-2</v>
+      </c>
+      <c r="F4" s="9">
+        <v>4.9558206288724801E-2</v>
+      </c>
+      <c r="G4" s="9">
+        <v>5.01049496748395E-2</v>
+      </c>
+      <c r="H4" s="9">
+        <v>5.0571633294625197E-2</v>
+      </c>
+      <c r="I4" s="9">
+        <v>5.10107148466186E-2</v>
+      </c>
+      <c r="J4" s="9">
+        <v>5.1434041444659198E-2</v>
+      </c>
+      <c r="K4" s="9">
+        <v>5.1801320035831898E-2</v>
+      </c>
+      <c r="L4" s="9">
+        <v>5.2096315032423797E-2</v>
+      </c>
+      <c r="M4" s="9">
+        <v>5.2380205672519303E-2</v>
+      </c>
+      <c r="N4" s="9">
+        <v>5.2647531736045299E-2</v>
+      </c>
+      <c r="O4" s="9">
+        <v>5.2896244885395599E-2</v>
+      </c>
+      <c r="P4" s="9">
+        <v>5.3135964996010102E-2</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>5.3346940945673903E-2</v>
+      </c>
+      <c r="R4" s="9">
+        <v>5.3530976418969797E-2</v>
+      </c>
+      <c r="S4" s="10">
+        <f t="shared" ref="S3:S15" si="0">(R4-H4)/H4</f>
+        <v>5.8517847487815314E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="9">
+        <v>3.5283825703161902E-2</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3.6715395009672698E-2</v>
+      </c>
+      <c r="D5" s="13">
+        <v>3.5997312302103998E-2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3.5997312302103998E-2</v>
+      </c>
+      <c r="F5" s="9">
+        <v>3.5304807000391597E-2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>3.4636548275199797E-2</v>
+      </c>
+      <c r="H5" s="9">
+        <v>3.39501683915008E-2</v>
+      </c>
+      <c r="I5" s="9">
+        <v>3.3281573297978401E-2</v>
+      </c>
+      <c r="J5" s="9">
+        <v>3.2636968474290103E-2</v>
+      </c>
+      <c r="K5" s="9">
+        <v>3.1989688226331803E-2</v>
+      </c>
+      <c r="L5" s="9">
+        <v>3.1330314759766602E-2</v>
+      </c>
+      <c r="M5" s="9">
+        <v>3.06957617753165E-2</v>
+      </c>
+      <c r="N5" s="9">
+        <v>3.00811822754267E-2</v>
+      </c>
+      <c r="O5" s="9">
+        <v>2.94840953327179E-2</v>
+      </c>
+      <c r="P5" s="9">
+        <v>2.8908598024567599E-2</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>2.8342792029388601E-2</v>
+      </c>
+      <c r="R5" s="9">
+        <v>2.7787053299524699E-2</v>
+      </c>
+      <c r="S5" s="10">
+        <f t="shared" si="0"/>
+        <v>-0.18153415384882143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1.3866633602674101E-3</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1.6109333596220101E-3</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1.47606050218053E-3</v>
+      </c>
+      <c r="E6" s="9">
+        <v>1.47606050218053E-3</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1.34599351244962E-3</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1.2204805372677599E-3</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1.0979568091240199E-3</v>
+      </c>
+      <c r="I6" s="9">
+        <v>9.7965274351189411E-4</v>
+      </c>
+      <c r="J6" s="9">
+        <v>8.6559361849834196E-4</v>
+      </c>
+      <c r="K6" s="9">
+        <v>7.5495561388647504E-4</v>
+      </c>
+      <c r="L6" s="9">
+        <v>6.4758284836130997E-4</v>
+      </c>
+      <c r="M6" s="9">
+        <v>5.4425186483300896E-4</v>
+      </c>
+      <c r="N6" s="9">
+        <v>4.4468734709879099E-4</v>
+      </c>
+      <c r="O6" s="9">
+        <v>3.4869808302601698E-4</v>
+      </c>
+      <c r="P6" s="9">
+        <v>2.5617962527078902E-4</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>1.66883783543993E-4</v>
+      </c>
+      <c r="R6" s="9">
+        <v>8.0738925815293907E-5</v>
+      </c>
+      <c r="S6" s="10">
+        <f t="shared" si="0"/>
+        <v>-0.92646438808489229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5.1947908548329999E-3</v>
+      </c>
+      <c r="C7" s="9">
+        <v>5.0770532380682697E-3</v>
+      </c>
+      <c r="D7" s="13">
+        <v>4.9430921827453402E-3</v>
+      </c>
+      <c r="E7" s="9">
+        <v>4.9430921827453402E-3</v>
+      </c>
+      <c r="F7" s="9">
+        <v>4.8139527150107197E-3</v>
+      </c>
+      <c r="G7" s="9">
+        <v>4.6893347866469801E-3</v>
+      </c>
+      <c r="H7" s="9">
+        <v>4.56433607542963E-3</v>
+      </c>
+      <c r="I7" s="9">
+        <v>4.5013499699016399E-3</v>
+      </c>
+      <c r="J7" s="9">
+        <v>4.4406239073833198E-3</v>
+      </c>
+      <c r="K7" s="9">
+        <v>4.3785621649348903E-3</v>
+      </c>
+      <c r="L7" s="9">
+        <v>4.3138572201904604E-3</v>
+      </c>
+      <c r="M7" s="9">
+        <v>4.2515879329379303E-3</v>
+      </c>
+      <c r="N7" s="9">
+        <v>4.1911356518326299E-3</v>
+      </c>
+      <c r="O7" s="9">
+        <v>4.1321977148234199E-3</v>
+      </c>
+      <c r="P7" s="9">
+        <v>4.0753908720161502E-3</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>4.0190774769251897E-3</v>
+      </c>
+      <c r="R7" s="9">
+        <v>3.9633313878154599E-3</v>
+      </c>
+      <c r="S7" s="10">
+        <f t="shared" si="0"/>
+        <v>-0.13167406555565672</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="9">
+        <v>4.51007615360981E-2</v>
+      </c>
+      <c r="C8" s="9">
+        <v>4.3538240914059098E-2</v>
+      </c>
+      <c r="D8" s="13">
+        <v>4.0377147041685803E-2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>4.0377147041685803E-2</v>
+      </c>
+      <c r="F8" s="9">
+        <v>3.7328787920488798E-2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>3.4387160505910001E-2</v>
+      </c>
+      <c r="H8" s="9">
+        <v>3.1508596468086299E-2</v>
+      </c>
+      <c r="I8" s="9">
+        <v>2.8727965824996399E-2</v>
+      </c>
+      <c r="J8" s="9">
+        <v>2.6047108692186301E-2</v>
+      </c>
+      <c r="K8" s="9">
+        <v>2.42354281728057E-2</v>
+      </c>
+      <c r="L8" s="9">
+        <v>2.3595194192137198E-2</v>
+      </c>
+      <c r="M8" s="9">
+        <v>2.2979060235009899E-2</v>
+      </c>
+      <c r="N8" s="9">
+        <v>2.2383107605520799E-2</v>
+      </c>
+      <c r="O8" s="9">
+        <v>2.18052534585602E-2</v>
+      </c>
+      <c r="P8" s="9">
+        <v>2.1248293521418299E-2</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>2.0703263581689502E-2</v>
+      </c>
+      <c r="R8" s="9">
+        <v>2.0170325096472E-2</v>
+      </c>
+      <c r="S8" s="10">
+        <f t="shared" si="0"/>
+        <v>-0.35984691933512003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1.44629210147961E-2</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1.3910542780015901E-2</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1.4220137469831E-2</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1.4220137469831E-2</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1.45187438243776E-2</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1.4806895122757799E-2</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1.5066883868955799E-2</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1.53142554304645E-2</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1.55527509015451E-2</v>
+      </c>
+      <c r="K9" s="9">
+        <v>1.57703192312224E-2</v>
+      </c>
+      <c r="L9" s="9">
+        <v>1.5961944068481601E-2</v>
+      </c>
+      <c r="M9" s="9">
+        <v>1.6146355663038299E-2</v>
+      </c>
+      <c r="N9" s="9">
+        <v>1.6322070178052501E-2</v>
+      </c>
+      <c r="O9" s="9">
+        <v>1.6488611140134401E-2</v>
+      </c>
+      <c r="P9" s="9">
+        <v>1.66491302681194E-2</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>1.6797578395370501E-2</v>
+      </c>
+      <c r="R9" s="9">
+        <v>1.69345939107097E-2</v>
+      </c>
+      <c r="S9" s="10">
+        <f t="shared" si="0"/>
+        <v>0.12396126883291236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="9">
+        <v>2.60868658707736E-2</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2.5091465557896299E-2</v>
+      </c>
+      <c r="D10" s="13">
+        <v>2.4595021621217499E-2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2.4595021621217499E-2</v>
+      </c>
+      <c r="F10" s="9">
+        <v>2.4116211221958901E-2</v>
+      </c>
+      <c r="G10" s="9">
+        <v>2.3654165334041698E-2</v>
+      </c>
+      <c r="H10" s="9">
+        <v>2.3179945971375199E-2</v>
+      </c>
+      <c r="I10" s="9">
+        <v>2.2718072267962901E-2</v>
+      </c>
+      <c r="J10" s="9">
+        <v>2.22727713376407E-2</v>
+      </c>
+      <c r="K10" s="9">
+        <v>2.1825838955700401E-2</v>
+      </c>
+      <c r="L10" s="9">
+        <v>2.13708532691387E-2</v>
+      </c>
+      <c r="M10" s="9">
+        <v>2.09329943925998E-2</v>
+      </c>
+      <c r="N10" s="9">
+        <v>2.05089463725374E-2</v>
+      </c>
+      <c r="O10" s="9">
+        <v>2.0097009144628E-2</v>
+      </c>
+      <c r="P10" s="9">
+        <v>1.9699966856760901E-2</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>1.9309703368911899E-2</v>
+      </c>
+      <c r="R10" s="9">
+        <v>1.8926470704058802E-2</v>
+      </c>
+      <c r="S10" s="10">
+        <f t="shared" si="0"/>
+        <v>-0.18349806649976635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="9">
+        <v>5.5668083466623497E-2</v>
+      </c>
+      <c r="C11" s="9">
+        <v>5.7776350391532498E-2</v>
+      </c>
+      <c r="D11" s="13">
+        <v>5.7927073756841301E-2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>5.7927073756841301E-2</v>
+      </c>
+      <c r="F11" s="9">
+        <v>5.80723564408233E-2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>5.8212552365605803E-2</v>
+      </c>
+      <c r="H11" s="9">
+        <v>5.8277345796159501E-2</v>
+      </c>
+      <c r="I11" s="9">
+        <v>5.83275138186473E-2</v>
+      </c>
+      <c r="J11" s="9">
+        <v>5.8375881731609701E-2</v>
+      </c>
+      <c r="K11" s="9">
+        <v>5.8376198711893902E-2</v>
+      </c>
+      <c r="L11" s="9">
+        <v>5.8310456348625202E-2</v>
+      </c>
+      <c r="M11" s="9">
+        <v>5.8247188693900803E-2</v>
+      </c>
+      <c r="N11" s="9">
+        <v>5.8179544560930503E-2</v>
+      </c>
+      <c r="O11" s="9">
+        <v>5.8104640280925102E-2</v>
+      </c>
+      <c r="P11" s="9">
+        <v>5.8032444410560602E-2</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>5.7940840343695003E-2</v>
+      </c>
+      <c r="R11" s="9">
+        <v>5.7831511555778398E-2</v>
+      </c>
+      <c r="S11" s="10">
+        <f t="shared" si="0"/>
+        <v>-7.6502152644447249E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="9">
+        <v>5.01683262158387E-2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>4.8942553419554398E-2</v>
+      </c>
+      <c r="D12" s="13">
+        <v>4.9017836183847301E-2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>4.9017836183847301E-2</v>
+      </c>
+      <c r="F12" s="9">
+        <v>4.90904686019095E-2</v>
+      </c>
+      <c r="G12" s="9">
+        <v>4.9160557952824001E-2</v>
+      </c>
+      <c r="H12" s="9">
+        <v>4.9168688482966703E-2</v>
+      </c>
+      <c r="I12" s="9">
+        <v>4.9166170017657503E-2</v>
+      </c>
+      <c r="J12" s="9">
+        <v>4.91637419189438E-2</v>
+      </c>
+      <c r="K12" s="9">
+        <v>4.9122400177978198E-2</v>
+      </c>
+      <c r="L12" s="9">
+        <v>4.9027020040477397E-2</v>
+      </c>
+      <c r="M12" s="9">
+        <v>4.8935230252174798E-2</v>
+      </c>
+      <c r="N12" s="9">
+        <v>4.8841195461002899E-2</v>
+      </c>
+      <c r="O12" s="9">
+        <v>4.8742431234250198E-2</v>
+      </c>
+      <c r="P12" s="9">
+        <v>4.8647238151682003E-2</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>4.8537019761176303E-2</v>
+      </c>
+      <c r="R12" s="9">
+        <v>4.8413157547805202E-2</v>
+      </c>
+      <c r="S12" s="10">
+        <f t="shared" si="0"/>
+        <v>-1.5366099004719974E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="9">
+        <v>3.5222740409149897E-2</v>
+      </c>
+      <c r="C13" s="9">
+        <v>3.9350890184148501E-2</v>
+      </c>
+      <c r="D13" s="13">
+        <v>4.3610745841196799E-2</v>
+      </c>
+      <c r="E13" s="9">
+        <v>4.3610745841196799E-2</v>
+      </c>
+      <c r="F13" s="9">
+        <v>4.7718731234100399E-2</v>
+      </c>
+      <c r="G13" s="9">
+        <v>5.1682884396510698E-2</v>
+      </c>
+      <c r="H13" s="9">
+        <v>5.5443483054485203E-2</v>
+      </c>
+      <c r="I13" s="9">
+        <v>5.9055797212069099E-2</v>
+      </c>
+      <c r="J13" s="9">
+        <v>6.2538495714070996E-2</v>
+      </c>
+      <c r="K13" s="9">
+        <v>6.5846155289318697E-2</v>
+      </c>
+      <c r="L13" s="9">
+        <v>6.8956161029791102E-2</v>
+      </c>
+      <c r="M13" s="9">
+        <v>7.1949098301825595E-2</v>
+      </c>
+      <c r="N13" s="9">
+        <v>7.4822820417572405E-2</v>
+      </c>
+      <c r="O13" s="9">
+        <v>7.7578675632137495E-2</v>
+      </c>
+      <c r="P13" s="9">
+        <v>8.0234883872831606E-2</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>8.2765367487161096E-2</v>
+      </c>
+      <c r="R13" s="9">
+        <v>8.5174817386557702E-2</v>
+      </c>
+      <c r="S13" s="10">
+        <f t="shared" si="0"/>
+        <v>0.53624578929961952</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1.5328670694862901E-2</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1.6550341974918201E-2</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1.7451522681676799E-2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1.7451522681676799E-2</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1.83205331359735E-2</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1.9159117067289001E-2</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1.9944690425740201E-2</v>
+      </c>
+      <c r="I14" s="9">
+        <v>2.069752678852E-2</v>
+      </c>
+      <c r="J14" s="9">
+        <v>2.1423350168914699E-2</v>
+      </c>
+      <c r="K14" s="9">
+        <v>2.2106038431750501E-2</v>
+      </c>
+      <c r="L14" s="9">
+        <v>2.2738296996887501E-2</v>
+      </c>
+      <c r="M14" s="9">
+        <v>2.3346755753260701E-2</v>
+      </c>
+      <c r="N14" s="9">
+        <v>2.39299721359078E-2</v>
+      </c>
+      <c r="O14" s="9">
+        <v>2.4487803699201598E-2</v>
+      </c>
+      <c r="P14" s="9">
+        <v>2.50254650347859E-2</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>2.5534347564824901E-2</v>
+      </c>
+      <c r="R14" s="9">
+        <v>2.6015665013880099E-2</v>
+      </c>
+      <c r="S14" s="10">
+        <f t="shared" si="0"/>
+        <v>0.30439051489637686</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="9">
+        <v>6.6809854973505306E-2</v>
+      </c>
+      <c r="C15" s="9">
+        <v>6.2245255791008203E-2</v>
+      </c>
+      <c r="D15" s="13">
+        <v>6.0548112478828797E-2</v>
+      </c>
+      <c r="E15" s="9">
+        <v>6.0548112478828797E-2</v>
+      </c>
+      <c r="F15" s="9">
+        <v>5.8911428240930201E-2</v>
+      </c>
+      <c r="G15" s="9">
+        <v>5.7332048964475101E-2</v>
+      </c>
+      <c r="H15" s="9">
+        <v>5.5739512034445299E-2</v>
+      </c>
+      <c r="I15" s="9">
+        <v>5.4193089181475702E-2</v>
+      </c>
+      <c r="J15" s="9">
+        <v>5.2702154473543102E-2</v>
+      </c>
+      <c r="K15" s="9">
+        <v>5.1223107017573898E-2</v>
+      </c>
+      <c r="L15" s="9">
+        <v>4.9741174759520702E-2</v>
+      </c>
+      <c r="M15" s="9">
+        <v>4.8315026173349901E-2</v>
+      </c>
+      <c r="N15" s="9">
+        <v>4.6936153162248702E-2</v>
+      </c>
+      <c r="O15" s="9">
+        <v>4.55999674548455E-2</v>
+      </c>
+      <c r="P15" s="9">
+        <v>4.4312095919235003E-2</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>4.3053637858884199E-2</v>
+      </c>
+      <c r="R15" s="9">
+        <v>4.18248216233724E-2</v>
+      </c>
+      <c r="S15" s="10">
+        <f t="shared" si="0"/>
+        <v>-0.24963782249249059</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B15">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:R15">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:S15">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R23"/>
   <sheetViews>
@@ -90216,7 +94285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
@@ -90562,7 +94631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>

</xml_diff>